<commit_message>
empty dataframe web version
</commit_message>
<xml_diff>
--- a/nlqs/nalir_nlidb_anp.nlqs.xlsx
+++ b/nlqs/nalir_nlidb_anp.nlqs.xlsx
@@ -9,21 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6770"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="2" r:id="rId1"/>
+    <sheet name="TD" sheetId="2" r:id="rId1"/>
     <sheet name="nalir_nlidb_anp.nlqs" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
-  </pivotCaches>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="112">
   <si>
     <t>NLQ</t>
   </si>
@@ -346,16 +343,19 @@
     <t>Workaround replacing gas production by oil production</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Observation</t>
   </si>
   <si>
-    <t>NLQ count</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>NaLIR</t>
+  </si>
+  <si>
+    <t>GLAMORISE</t>
+  </si>
+  <si>
+    <t>Final Result</t>
+  </si>
+  <si>
+    <t>status/NLIDB</t>
   </si>
 </sst>
 </file>
@@ -839,14 +839,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -892,7 +887,11 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -905,310 +904,37 @@
 </styleSheet>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Alexandre Novello" refreshedDate="44232.847868287034" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="26">
-  <cacheSource type="worksheet">
-    <worksheetSource name="Tabela1"/>
-  </cacheSource>
-  <cacheFields count="6">
-    <cacheField name="NLQ" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="NLQ preproccessed by GLAMORISE" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="NLIDB SQL" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="GLAMORISE SQL" numFmtId="0">
-      <sharedItems longText="1"/>
-    </cacheField>
-    <cacheField name="Status" numFmtId="0">
-      <sharedItems count="2">
-        <s v="success"/>
-        <s v="failure"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Observation" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:E4" totalsRowShown="0">
+  <tableColumns count="4">
+    <tableColumn id="1" name="status/NLIDB"/>
+    <tableColumn id="2" name="GLAMORISE">
+      <calculatedColumnFormula>COUNTIF(Tabela1[GLAMORISE],TD!$B3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="NaLIR">
+      <calculatedColumnFormula>COUNTIF(Tabela1[NaLIR],TD!$B3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Final Result">
+      <calculatedColumnFormula>COUNTIF(Tabela1[Final Result],TD!$B3)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="26">
-  <r>
-    <s v="What was the production of oil in the state of Rio de Janeiro?"/>
-    <s v="What was the production of oil in the state of Rio de Janeiro?"/>
-    <s v="SELECT oil_production FROM ANP WHERE lower(state) = 'rio de janeiro'"/>
-    <s v="SELECT * FROM NLIDB_RESULT_SET"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the average monthly production of oil in the state of Rio de Janeiro?"/>
-    <s v="What was the month production of oil in the state of Rio de Janeiro?"/>
-    <s v="SELECT year, month, oil_production FROM ANP WHERE lower(state) = 'rio de janeiro'"/>
-    <s v="SELECT AVG(anp_oil_production) as avg_anp_oil_production FROM (SELECT SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_year, anp_month)"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the average yearly production of oil in the state of Alagoas?"/>
-    <s v="What was the year production of oil in the state of Alagoas?"/>
-    <s v="SELECT year, oil_production FROM ANP WHERE lower(state) = 'alagoas'"/>
-    <s v="SELECT AVG(anp_oil_production) as avg_anp_oil_production FROM (SELECT SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_year)"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="How many fields are there in ParanÃ¡?"/>
-    <s v="How many fields are there in ParanÃ¡?"/>
-    <s v="SELECT distinct field FROM ANP WHERE lower(state) = 'paranÃ¡'"/>
-    <s v="SELECT count(anp_field) as count_anp_field FROM NLIDB_RESULT_SET"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the maximum production of oil in the state of CearÃ¡ per field?"/>
-    <s v="What was the production of oil in the state of CearÃ¡ per field?"/>
-    <s v="SELECT oil_production, field FROM ANP WHERE lower(state) = 'cearÃ¡'"/>
-    <s v="SELECT anp_field, max(anp_oil_production) as max_anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_field ORDER BY anp_field"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the minimum gas production in the state of SÃ£o Paulo per basin?"/>
-    <s v="What was the gas production in the state of SÃ£o Paulo per basin?"/>
-    <s v="SELECT gas_production, basin FROM ANP WHERE lower(state) = 'sÃ£o paulo'"/>
-    <s v="SELECT anp_basin, min(anp_gas_production) as min_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_basin ORDER BY anp_basin"/>
-    <x v="1"/>
-    <s v="Attribute oil production found wrongly. Difficulty matching gas production"/>
-  </r>
-  <r>
-    <s v="What was the average monthly oil production by the operator PetrobrÃ¡s?"/>
-    <s v="What was the month oil production by the operator PetrobrÃ¡s?"/>
-    <s v="SELECT year, month, oil_production, operator FROM ANP WHERE lower(operator) = 'petrobras'"/>
-    <s v="select anp_operator, avg(anp_oil_production) as avg_anp_oil_production from (select anp_operator, sum(anp_oil_production) as anp_oil_production from nlidb_result_set group by anp_operator, anp_year, anp_month) group by anp_operator order by anp_operator"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the mean yearly gas production per field?"/>
-    <s v="What was the year gas production per field?"/>
-    <s v="SELECT year, gas_production, field FROM ANP "/>
-    <s v="SELECT anp_field, AVG(anp_gas_production) as avg_anp_gas_production FROM (SELECT anp_field, SUM(anp_gas_production) as anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_year) GROUP BY anp_field ORDER BY anp_field"/>
-    <x v="1"/>
-    <s v="Attribute oil production found wrongly. Difficulty matching gas production"/>
-  </r>
-  <r>
-    <s v="What was the mean gas production per month per field?"/>
-    <s v="What was the gas production per month per field?"/>
-    <s v="SELECT gas_production, year, month, field FROM ANP "/>
-    <s v="SELECT anp_year, anp_month, anp_field, AVG(anp_gas_production) as avg_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_year, anp_month, anp_field ORDER BY anp_year, anp_month, anp_field"/>
-    <x v="1"/>
-    <s v="Attribute oil production found wrongly. Difficulty matching gas production"/>
-  </r>
-  <r>
-    <s v="What was the per month mean gas production per field?"/>
-    <s v="What was the per month gas production per field?"/>
-    <s v="SELECT year, month, gas_production, field FROM ANP "/>
-    <s v="SELECT anp_year, anp_month, anp_field, AVG(anp_gas_production) as avg_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_year, anp_month, anp_field ORDER BY anp_year, anp_month, anp_field"/>
-    <x v="1"/>
-    <s v="Attribute oil production found wrongly. Difficulty matching gas production"/>
-  </r>
-  <r>
-    <s v="What was the per field mean gas production per month?"/>
-    <s v="What was the per field gas production per month?"/>
-    <s v="SELECT field, gas_production, year, month FROM ANP "/>
-    <s v="SELECT anp_field, anp_year, anp_month, AVG(anp_gas_production) as avg_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_year, anp_month ORDER BY anp_field, anp_year, anp_month"/>
-    <x v="1"/>
-    <s v="Attribute oil production found wrongly. Difficulty matching gas production"/>
-  </r>
-  <r>
-    <s v="What was the mean monthly petroleum production by field in the state of Rio de Janeiro?"/>
-    <s v="What was the month petroleum production by field in the state of Rio de Janeiro?"/>
-    <s v="SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = 'rio de janeiro'"/>
-    <s v="SELECT anp_field, AVG(anp_oil_production) as avg_anp_oil_production FROM (SELECT anp_field, SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_year, anp_month) GROUP BY anp_field ORDER BY anp_field"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the mean yearly petroleum production by field by Rio de Janeiro?"/>
-    <s v="What was the year petroleum production by field by Rio de Janeiro?"/>
-    <s v="SELECT year, field, oil_production FROM ANP WHERE lower(state) = 'rio de janeiro'"/>
-    <s v="SELECT anp_field, AVG(anp_oil_production) as avg_anp_oil_production FROM (SELECT anp_field, SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_year) GROUP BY anp_field ORDER BY anp_field"/>
-    <x v="1"/>
-    <s v="Erroneously identified state attribute"/>
-  </r>
-  <r>
-    <s v="What was the mean gas production per field with production greater than 100 cubic meters?"/>
-    <s v="What was the gas production per field with production greater than 100 cubic meters?"/>
-    <s v="SELECT gas_production, field FROM ANP WHERE gas_production &gt; 100"/>
-    <s v="SELECT anp_field, avg(anp_gas_production) as avg_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_field HAVING avg(anp_gas_production) &gt; 100 ORDER BY anp_field"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the mean gas production per basin with production less than 1000 cubic meters?"/>
-    <s v="What was the gas production per basin with production less than 1000 cubic meters?"/>
-    <s v="SELECT gas_production, basin FROM ANP WHERE gas_production &lt; 1000"/>
-    <s v="SELECT anp_basin, avg(anp_gas_production) as avg_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_basin HAVING avg(anp_gas_production) &lt; 1000 ORDER BY anp_basin"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Which field produces the most oil per month?"/>
-    <s v="Which field produces the oil per month?"/>
-    <s v="SELECT field, oil_production, year, month FROM ANP "/>
-    <s v="SELECT anp_year, anp_month, anp_field, max(anp_oil_production) as max_anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_year, anp_month, anp_field ORDER BY anp_year, anp_month, anp_field"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Which basin has the highest yearly oil production?"/>
-    <s v="Which basin has the year oil production?"/>
-    <s v="SELECT basin, year, oil_production FROM ANP "/>
-    <s v="SELECT anp_basin, max(anp_oil_production) as max_anp_oil_production FROM (SELECT anp_basin, SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_basin, anp_year) GROUP BY anp_basin ORDER BY anp_basin"/>
-    <x v="1"/>
-    <s v="Attribute basin not identified. Tried to change the field, but there was no workaround"/>
-  </r>
-  <r>
-    <s v="Which federated state has the lowest gas production?"/>
-    <s v="Which federated state has the gas production?"/>
-    <s v="SELECT state, gas_production FROM ANP "/>
-    <s v="SELECT anp_state, min(anp_gas_production) as min_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_state ORDER BY anp_state"/>
-    <x v="1"/>
-    <s v="Attribute basin not identified. Tried to change the field, but there was no workaround"/>
-  </r>
-  <r>
-    <s v="Which state of the federation has the lowest gas production?"/>
-    <s v="Which state of the federation has the gas production?"/>
-    <s v="SELECT state, gas_production FROM ANP "/>
-    <s v="SELECT anp_state, min(anp_gas_production) as min_anp_gas_production FROM NLIDB_RESULT_SET GROUP BY anp_state ORDER BY anp_state"/>
-    <x v="1"/>
-    <s v="Attribute state not identified. Tried to change the field, but there was no workaround"/>
-  </r>
-  <r>
-    <s v="What was the average yearly production of oil per field and state in the year in 2015?"/>
-    <s v="What was the year production of oil per field and state in the year in 2015?"/>
-    <s v="SELECT year, oil_production, field, state FROM ANP WHERE year = 2015"/>
-    <s v="SELECT anp_field, anp_state, AVG(anp_oil_production) as avg_anp_oil_production FROM (SELECT anp_field, anp_state, SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_state, anp_year) GROUP BY anp_field, anp_state ORDER BY anp_field, anp_state"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the average monthly production of oil per field in the state of Rio de Janeiro and year 2015?"/>
-    <s v="What was the month production of oil per field in the state of Rio de Janeiro and year 2015?"/>
-    <s v="SELECT year, month, field, oil_production FROM ANP WHERE lower(state) = 'rio de janeiro' and year = 2015"/>
-    <s v="SELECT anp_field, AVG(anp_oil_production) as avg_anp_oil_production FROM (SELECT anp_field, SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_year, anp_month) GROUP BY anp_field ORDER BY anp_field"/>
-    <x v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="What was the minimum oil production in the state of SÃ£o Paulo per basin?"/>
-    <s v="What was the oil production in the state of SÃ£o Paulo per basin?"/>
-    <s v="SELECT oil_production, basin FROM ANP WHERE lower(state) = 'sÃ£o paulo'"/>
-    <s v="SELECT anp_basin, min(anp_oil_production) as min_anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_basin ORDER BY anp_basin"/>
-    <x v="0"/>
-    <s v="Workaround replacing gas production by oil production"/>
-  </r>
-  <r>
-    <s v="What was the mean yearly oil production per field?"/>
-    <s v="What was the year oil production per field?"/>
-    <s v="SELECT year, oil_production, field FROM ANP "/>
-    <s v="SELECT anp_field, AVG(anp_oil_production) as avg_anp_oil_production FROM (SELECT anp_field, SUM(anp_oil_production) as anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_year) GROUP BY anp_field ORDER BY anp_field"/>
-    <x v="0"/>
-    <s v="Workaround replacing gas production by oil production"/>
-  </r>
-  <r>
-    <s v="What was the mean oil production per month per field?"/>
-    <s v="What was the oil production per month per field?"/>
-    <s v="SELECT oil_production, year, month, field FROM ANP "/>
-    <s v="SELECT anp_year, anp_month, anp_field, AVG(anp_oil_production) as avg_anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_year, anp_month, anp_field ORDER BY anp_year, anp_month, anp_field"/>
-    <x v="0"/>
-    <s v="Workaround replacing gas production by oil production"/>
-  </r>
-  <r>
-    <s v="What was the per month mean oil production per field?"/>
-    <s v="What was the per month oil production per field?"/>
-    <s v="SELECT year, month, oil_production, field FROM ANP "/>
-    <s v="SELECT anp_year, anp_month, anp_field, AVG(anp_oil_production) as avg_anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_year, anp_month, anp_field ORDER BY anp_year, anp_month, anp_field"/>
-    <x v="0"/>
-    <s v="Workaround replacing gas production by oil production"/>
-  </r>
-  <r>
-    <s v="What was the per field mean oil production per month?"/>
-    <s v="What was the per field oil production per month?"/>
-    <s v="SELECT field, oil_production, year, month FROM ANP "/>
-    <s v="SELECT anp_field, anp_year, anp_month, AVG(anp_oil_production) as avg_anp_oil_production FROM NLIDB_RESULT_SET GROUP BY anp_field, anp_year, anp_month ORDER BY anp_field, anp_year, anp_month"/>
-    <x v="0"/>
-    <s v="Workaround replacing gas production by oil production"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Status">
-  <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="NLQ count" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F27" totalsRowShown="0">
-  <autoFilter ref="A1:F27"/>
-  <tableColumns count="6">
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H27" totalsRowShown="0">
+  <autoFilter ref="A1:H27"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="NLQ"/>
     <tableColumn id="2" name="NLQ preproccessed by GLAMORISE"/>
     <tableColumn id="3" name="NLIDB SQL"/>
     <tableColumn id="4" name="GLAMORISE SQL"/>
-    <tableColumn id="5" name="Status"/>
+    <tableColumn id="8" name="GLAMORISE"/>
+    <tableColumn id="9" name="NaLIR"/>
+    <tableColumn id="7" name="Final Result" dataDxfId="0">
+      <calculatedColumnFormula>Tabela1[[#This Row],[NaLIR]]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="6" name="Observation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1478,74 +1204,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B6"/>
+  <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="A3:B6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>107</v>
-      </c>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIF(Tabela1[GLAMORISE],TD!$B3)</f>
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <f>COUNTIF(Tabela1[NaLIR],TD!$B3)</f>
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <f>COUNTIF(Tabela1[Final Result],TD!$B3)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="4">
+      <c r="C4">
+        <f>COUNTIF(Tabela1[GLAMORISE],TD!$B4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIF(Tabela1[NaLIR],TD!$B4)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="4">
-        <v>26</v>
+      <c r="E4">
+        <f>COUNTIF(Tabela1[Final Result],TD!$B4)</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="206.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="93.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="206.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.7265625" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1559,13 +1306,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1581,8 +1334,15 @@
       <c r="E2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1598,8 +1358,15 @@
       <c r="E3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1615,8 +1382,15 @@
       <c r="E4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1632,8 +1406,15 @@
       <c r="E5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1649,8 +1430,15 @@
       <c r="E6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1663,14 +1451,21 @@
       <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1686,8 +1481,15 @@
       <c r="E8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1700,14 +1502,21 @@
       <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1720,14 +1529,21 @@
       <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1740,14 +1556,21 @@
       <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1760,14 +1583,21 @@
       <c r="D12" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1783,8 +1613,15 @@
       <c r="E13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1797,14 +1634,21 @@
       <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1820,8 +1664,15 @@
       <c r="E15" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1837,8 +1688,15 @@
       <c r="E16" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1854,8 +1712,15 @@
       <c r="E17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1868,14 +1733,21 @@
       <c r="D18" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1888,14 +1760,21 @@
       <c r="D19" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1908,14 +1787,21 @@
       <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>failure</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1931,8 +1817,15 @@
       <c r="E21" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1948,8 +1841,15 @@
       <c r="E22" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1966,10 +1866,17 @@
         <v>85</v>
       </c>
       <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+      <c r="H23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1986,10 +1893,17 @@
         <v>85</v>
       </c>
       <c r="F24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+      <c r="H24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -2006,10 +1920,17 @@
         <v>85</v>
       </c>
       <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+      <c r="H25" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -2026,10 +1947,17 @@
         <v>85</v>
       </c>
       <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+      <c r="H26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -2046,6 +1974,13 @@
         <v>85</v>
       </c>
       <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
+      </c>
+      <c r="H27" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DANKE adjustments and ANP NLQs
</commit_message>
<xml_diff>
--- a/nlqs/nalir_nlidb_anp.nlqs.xlsx
+++ b/nlqs/nalir_nlidb_anp.nlqs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765"/>
   </bookViews>
   <sheets>
     <sheet name="TD" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="276">
   <si>
     <t>NLQ</t>
   </si>
@@ -870,12 +870,36 @@
   <si>
     <t>D</t>
   </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">%  </t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Give me the operator with the highest number of fields</t>
+  </si>
+  <si>
+    <t>Give me the operator with the fields</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ANP.OPERATOR as ANP_OPERATOR, ANP.FIELD as ANP_FIELD FROM ANP</t>
+  </si>
+  <si>
+    <t>SELECT anp_operator, max(ANP_FIELD) as max_ANP_FIELD FROM (SELECT anp_operator, count(DISTINCT ANP_FIELD) as ANP_FIELD FROM NLIDB_result_set GROUP BY anp_operator) ORDER BY anp_operator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1032,6 +1056,12 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1402,7 +1432,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1445,8 +1475,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1497,13 +1528,13 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1515,8 +1546,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1550,6 +1588,7 @@
     <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Porcentagem" xfId="42" builtinId="5"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1560,7 +1599,140 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1587,17 +1759,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:E4" totalsRowShown="0">
-  <tableColumns count="4">
-    <tableColumn id="1" name="status/NLIDB"/>
-    <tableColumn id="2" name="GLAMORISE">
-      <calculatedColumnFormula>COUNTIF(Tabela1[GLAMORISE],TD!$B3)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:H5" totalsRowCount="1" headerRowDxfId="3">
+  <tableColumns count="7">
+    <tableColumn id="1" name="status/NLIDB" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="GLAMORISE" totalsRowFunction="sum" dataDxfId="8">
+      <calculatedColumnFormula>COUNTIF(nalir_nlidb_anp.nlqs!$E$2:$E$22,TD!$B3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="NaLIR">
-      <calculatedColumnFormula>COUNTIF(Tabela1[NaLIR],TD!$B3)</calculatedColumnFormula>
+    <tableColumn id="5" name="%" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="5" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>C3/(C$3+C$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Final Result">
-      <calculatedColumnFormula>COUNTIF(Tabela1[Final Result],TD!$B3)</calculatedColumnFormula>
+    <tableColumn id="3" name="NaLIR" totalsRowFunction="sum" dataDxfId="7">
+      <calculatedColumnFormula>COUNTIF(nalir_nlidb_anp.nlqs!$F$2:$F$22,TD!$B3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="% " totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="4" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>E3/(E$3+E$4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Final Result" totalsRowFunction="sum" dataDxfId="6">
+      <calculatedColumnFormula>COUNTIF(nalir_nlidb_anp.nlqs!$G$2:$G$22,TD!$B3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="%  " totalsRowFunction="sum" dataDxfId="12">
+      <calculatedColumnFormula>G3/(G$3+G$4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1605,17 +1786,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela24" displayName="Tabela24" ref="B7:E9" totalsRowShown="0">
-  <tableColumns count="4">
-    <tableColumn id="1" name="status/NLIDB"/>
-    <tableColumn id="2" name="GLAMORISE" dataDxfId="2">
-      <calculatedColumnFormula>COUNTIF(DANKE!E:E,TD!$B8)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela24" displayName="Tabela24" ref="B8:H11" totalsRowCount="1" headerRowDxfId="2">
+  <tableColumns count="7">
+    <tableColumn id="1" name="status/NLIDB" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="GLAMORISE" totalsRowFunction="sum" dataDxfId="18">
+      <calculatedColumnFormula>COUNTIF(DANKE!E:E,TD!$B9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="DANKE" dataDxfId="1">
-      <calculatedColumnFormula>COUNTIF(DANKE!F:F,TD!$B8)</calculatedColumnFormula>
+    <tableColumn id="5" name="%" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="1" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>C9/(C$3+C$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Final Result" dataDxfId="0">
+    <tableColumn id="3" name="DANKE" totalsRowFunction="sum" dataDxfId="17">
+      <calculatedColumnFormula>COUNTIF(DANKE!F:F,TD!$B9)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="% " totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="0" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>E9/(E$3+E$4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Final Result" totalsRowFunction="sum" dataDxfId="16">
       <calculatedColumnFormula>Tabela24[[#This Row],[DANKE]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="%  " totalsRowFunction="sum" dataDxfId="9" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>G9/(G$3+G$4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1623,8 +1813,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H27" totalsRowShown="0">
-  <autoFilter ref="A1:H27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H28" totalsRowShown="0">
+  <autoFilter ref="A1:H28"/>
   <tableColumns count="8">
     <tableColumn id="1" name="NLQ"/>
     <tableColumn id="2" name="NLQ preproccessed by GLAMORISE"/>
@@ -1632,7 +1822,7 @@
     <tableColumn id="4" name="GLAMORISE SQL"/>
     <tableColumn id="8" name="GLAMORISE"/>
     <tableColumn id="9" name="NaLIR"/>
-    <tableColumn id="7" name="Final Result" dataDxfId="3">
+    <tableColumn id="7" name="Final Result" dataDxfId="15">
       <calculatedColumnFormula>Tabela1[[#This Row],[NaLIR]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="Observation"/>
@@ -1904,114 +2094,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E9" sqref="B7:E9"/>
+      <selection activeCell="H5" sqref="B2:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="7.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="2:8">
+      <c r="B2" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="G2" s="28" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H2" s="28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3" t="s">
         <v>85</v>
       </c>
       <c r="C3">
-        <f>COUNTIF(Tabela1[GLAMORISE],TD!$B3)</f>
-        <v>26</v>
-      </c>
-      <c r="D3">
-        <f>COUNTIF(Tabela1[NaLIR],TD!$B3)</f>
-        <v>17</v>
+        <f>COUNTIF(nalir_nlidb_anp.nlqs!$E$2:$E$22,TD!$B3)</f>
+        <v>21</v>
+      </c>
+      <c r="D3" s="24">
+        <f t="shared" ref="D3:D4" si="0">C3/(C$3+C$4)</f>
+        <v>1</v>
       </c>
       <c r="E3">
-        <f>COUNTIF(Tabela1[Final Result],TD!$B3)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+        <f>COUNTIF(nalir_nlidb_anp.nlqs!$F$2:$F$22,TD!$B3)</f>
+        <v>12</v>
+      </c>
+      <c r="F3" s="26">
+        <f t="shared" ref="F3:F4" si="1">E3/(E$3+E$4)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G3">
+        <f>COUNTIF(nalir_nlidb_anp.nlqs!$G$2:$G$22,TD!$B3)</f>
+        <v>12</v>
+      </c>
+      <c r="H3" s="24">
+        <f t="shared" ref="H3:H4" si="2">G3/(G$3+G$4)</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>86</v>
       </c>
       <c r="C4">
-        <f>COUNTIF(Tabela1[GLAMORISE],TD!$B4)</f>
+        <f>COUNTIF(nalir_nlidb_anp.nlqs!$E$2:$E$22,TD!$B4)</f>
         <v>0</v>
       </c>
-      <c r="D4">
-        <f>COUNTIF(Tabela1[NaLIR],TD!$B4)</f>
+      <c r="D4" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>COUNTIF(nalir_nlidb_anp.nlqs!$F$2:$F$22,TD!$B4)</f>
         <v>9</v>
       </c>
-      <c r="E4">
-        <f>COUNTIF(Tabela1[Final Result],TD!$B4)</f>
+      <c r="F4" s="24">
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G4">
+        <f>COUNTIF(nalir_nlidb_anp.nlqs!$G$2:$G$22,TD!$B4)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+      <c r="H4" s="25">
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5">
+        <f>SUBTOTAL(109,Tabela2[GLAMORISE])</f>
+        <v>21</v>
+      </c>
+      <c r="D5" s="25">
+        <f>SUBTOTAL(109,Tabela2[%])</f>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>SUBTOTAL(109,Tabela2[NaLIR])</f>
+        <v>21</v>
+      </c>
+      <c r="F5" s="27">
+        <f>SUBTOTAL(109,Tabela2[% ])</f>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f>SUBTOTAL(109,Tabela2[Final Result])</f>
+        <v>21</v>
+      </c>
+      <c r="H5" s="25">
+        <f>SUBTOTAL(109,Tabela2[%  ])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F8" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="G8" s="28" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8">
-        <f>COUNTIF(DANKE!E:E,TD!$B8)</f>
+      <c r="H8" s="28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9">
+        <f>COUNTIF(DANKE!E:E,TD!$B9)</f>
         <v>21</v>
       </c>
-      <c r="D8">
-        <f>COUNTIF(DANKE!F:F,TD!$B8)</f>
+      <c r="D9" s="24">
+        <f t="shared" ref="D9" si="3">C9/(C$3+C$4)</f>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>COUNTIF(DANKE!F:F,TD!$B9)</f>
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="F9" s="24">
+        <f t="shared" ref="F9" si="4">E9/(E$3+E$4)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G9">
         <f>Tabela24[[#This Row],[DANKE]]</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+      <c r="H9" s="24">
+        <f t="shared" ref="H9" si="5">G9/(G$3+G$4)</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
         <v>86</v>
       </c>
-      <c r="C9">
-        <f>COUNTIF(DANKE!E:E,TD!$B9)</f>
+      <c r="C10">
+        <f>COUNTIF(DANKE!E:E,TD!$B10)</f>
         <v>0</v>
       </c>
-      <c r="D9">
-        <f>COUNTIF(DANKE!F:F,TD!$B9)</f>
+      <c r="D10" s="24">
+        <f t="shared" ref="D10" si="6">C10/(C$3+C$4)</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>COUNTIF(DANKE!F:F,TD!$B10)</f>
         <v>9</v>
       </c>
-      <c r="E9">
+      <c r="F10" s="24">
+        <f t="shared" ref="F10" si="7">E10/(E$3+E$4)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G10">
         <f>Tabela24[[#This Row],[DANKE]]</f>
         <v>9</v>
+      </c>
+      <c r="H10" s="24">
+        <f t="shared" ref="H10" si="8">G10/(G$3+G$4)</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11">
+        <f>SUBTOTAL(109,Tabela24[GLAMORISE])</f>
+        <v>21</v>
+      </c>
+      <c r="D11" s="27">
+        <f>SUBTOTAL(109,Tabela24[%])</f>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f>SUBTOTAL(109,Tabela24[DANKE])</f>
+        <v>21</v>
+      </c>
+      <c r="F11" s="27">
+        <f>SUBTOTAL(109,Tabela24[% ])</f>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f>SUBTOTAL(109,Tabela24[Final Result])</f>
+        <v>21</v>
+      </c>
+      <c r="H11" s="25">
+        <f>SUBTOTAL(109,Tabela24[%  ])</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2031,15 +2346,15 @@
       <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="88.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="171.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="84.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="171.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="84.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="A1" s="2"/>
       <c r="E1" t="s">
         <v>266</v>
@@ -2048,7 +2363,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>112</v>
@@ -2066,37 +2381,37 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>116</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="5"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="30">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -2116,7 +2431,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7" s="5"/>
       <c r="B7" s="7" t="s">
         <v>121</v>
@@ -2126,7 +2441,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
         <v>119</v>
       </c>
@@ -2138,7 +2453,7 @@
       </c>
       <c r="D8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9" s="11"/>
       <c r="B9" s="7" t="s">
         <v>123</v>
@@ -2150,7 +2465,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10" s="11"/>
       <c r="B10" s="7" t="s">
         <v>124</v>
@@ -2160,7 +2475,7 @@
       </c>
       <c r="D10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11" s="11"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
@@ -2168,19 +2483,19 @@
       </c>
       <c r="D11" s="14"/>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6">
       <c r="A12" s="11"/>
       <c r="B12" s="13"/>
       <c r="C12" s="7"/>
       <c r="D12" s="14"/>
     </row>
-    <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1">
       <c r="A13" s="12"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -2200,7 +2515,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15" s="5"/>
       <c r="B15" s="7" t="s">
         <v>133</v>
@@ -2212,7 +2527,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -2224,7 +2539,7 @@
       </c>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" s="11"/>
       <c r="B17" s="7" t="s">
         <v>135</v>
@@ -2234,7 +2549,7 @@
       </c>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" s="11"/>
       <c r="B18" s="7" t="s">
         <v>136</v>
@@ -2244,7 +2559,7 @@
       </c>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" s="11"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -2252,23 +2567,23 @@
       </c>
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6">
       <c r="A20" s="11"/>
       <c r="B20" s="13"/>
       <c r="C20" s="7"/>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15.75" thickBot="1">
       <c r="A21" s="12"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="18" t="s">
         <v>146</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -2284,19 +2599,19 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" s="5"/>
-      <c r="B23" s="18"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="7" t="s">
         <v>148</v>
       </c>
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="18"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="7" t="s">
         <v>140</v>
       </c>
@@ -2304,9 +2619,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="A25" s="11"/>
-      <c r="B25" s="18"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="7" t="s">
         <v>149</v>
       </c>
@@ -2314,31 +2629,31 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" s="11"/>
-      <c r="B26" s="18"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="7"/>
       <c r="D26" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" s="11"/>
-      <c r="B27" s="18"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="13"/>
       <c r="D27" s="9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="30.75" thickBot="1">
       <c r="A28" s="12"/>
-      <c r="B28" s="19"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="8"/>
       <c r="D28" s="15" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
         <v>156</v>
       </c>
@@ -2358,7 +2673,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6">
       <c r="A30" s="5"/>
       <c r="B30" s="7" t="s">
         <v>148</v>
@@ -2368,7 +2683,7 @@
       </c>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6">
       <c r="A31" s="5" t="s">
         <v>157</v>
       </c>
@@ -2382,7 +2697,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6">
       <c r="A32" s="11"/>
       <c r="B32" s="7" t="s">
         <v>160</v>
@@ -2394,19 +2709,19 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6">
       <c r="A33" s="11"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="14"/>
     </row>
-    <row r="34" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" ht="15.75" thickBot="1">
       <c r="A34" s="12"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
         <v>165</v>
       </c>
@@ -2426,7 +2741,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6">
       <c r="A36" s="5"/>
       <c r="B36" s="7" t="s">
         <v>168</v>
@@ -2436,7 +2751,7 @@
       </c>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6">
       <c r="A37" s="5" t="s">
         <v>166</v>
       </c>
@@ -2450,7 +2765,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6">
       <c r="A38" s="11"/>
       <c r="B38" s="7" t="s">
         <v>170</v>
@@ -2462,31 +2777,31 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6">
       <c r="A39" s="11"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6">
       <c r="A40" s="11"/>
       <c r="B40" s="14"/>
       <c r="C40" s="13"/>
       <c r="D40" s="14"/>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6">
       <c r="A41" s="11"/>
       <c r="B41" s="7"/>
       <c r="C41" s="13"/>
       <c r="D41" s="14"/>
     </row>
-    <row r="42" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" ht="15.75" thickBot="1">
       <c r="A42" s="12"/>
       <c r="B42" s="16"/>
       <c r="C42" s="8"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
         <v>175</v>
       </c>
@@ -2506,7 +2821,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6">
       <c r="A44" s="5"/>
       <c r="B44" s="7" t="s">
         <v>121</v>
@@ -2518,7 +2833,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6">
       <c r="A45" s="5" t="s">
         <v>176</v>
       </c>
@@ -2530,7 +2845,7 @@
       </c>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6">
       <c r="A46" s="11"/>
       <c r="B46" s="7" t="s">
         <v>179</v>
@@ -2540,7 +2855,7 @@
       </c>
       <c r="D46" s="14"/>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6">
       <c r="A47" s="11"/>
       <c r="B47" s="7" t="s">
         <v>180</v>
@@ -2550,7 +2865,7 @@
       </c>
       <c r="D47" s="14"/>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6">
       <c r="A48" s="11"/>
       <c r="B48" s="7" t="s">
         <v>181</v>
@@ -2560,19 +2875,19 @@
       </c>
       <c r="D48" s="14"/>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6">
       <c r="A49" s="11"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="14"/>
     </row>
-    <row r="50" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" ht="15.75" thickBot="1">
       <c r="A50" s="12"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6">
       <c r="A51" s="5" t="s">
         <v>22</v>
       </c>
@@ -2590,7 +2905,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6">
       <c r="A52" s="5"/>
       <c r="B52" s="7" t="s">
         <v>121</v>
@@ -2600,7 +2915,7 @@
       </c>
       <c r="D52" s="9"/>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6">
       <c r="A53" s="5" t="s">
         <v>189</v>
       </c>
@@ -2614,7 +2929,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6">
       <c r="A54" s="11"/>
       <c r="B54" s="7" t="s">
         <v>179</v>
@@ -2624,7 +2939,7 @@
       </c>
       <c r="D54" s="14"/>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6">
       <c r="A55" s="11"/>
       <c r="B55" s="7" t="s">
         <v>192</v>
@@ -2634,7 +2949,7 @@
       </c>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6">
       <c r="A56" s="11"/>
       <c r="B56" s="7" t="s">
         <v>193</v>
@@ -2642,7 +2957,7 @@
       <c r="C56" s="7"/>
       <c r="D56" s="14"/>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6">
       <c r="A57" s="11"/>
       <c r="B57" s="7" t="s">
         <v>160</v>
@@ -2650,26 +2965,26 @@
       <c r="C57" s="13"/>
       <c r="D57" s="14"/>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6">
       <c r="A58" s="11"/>
       <c r="B58" s="7"/>
       <c r="C58" s="13"/>
       <c r="D58" s="14"/>
     </row>
-    <row r="59" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" ht="15.75" thickBot="1">
       <c r="A59" s="12"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6">
       <c r="A60" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="18" t="s">
         <v>204</v>
       </c>
       <c r="D60" s="21" t="s">
@@ -2682,52 +2997,52 @@
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6">
       <c r="A61" s="5"/>
       <c r="B61" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C61" s="18"/>
+      <c r="C61" s="19"/>
       <c r="D61" s="22"/>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6">
       <c r="A62" s="5" t="s">
         <v>200</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C62" s="18"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="22"/>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6">
       <c r="A63" s="11"/>
       <c r="B63" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C63" s="18"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="22"/>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6">
       <c r="A64" s="11"/>
       <c r="B64" s="7"/>
-      <c r="C64" s="18"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="22"/>
     </row>
-    <row r="65" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" ht="15.75" thickBot="1">
       <c r="A65" s="12"/>
       <c r="B65" s="8"/>
-      <c r="C65" s="19"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="23"/>
     </row>
-    <row r="66" spans="1:6" ht="309.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="309.60000000000002" customHeight="1">
       <c r="A66" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="18" t="s">
         <v>204</v>
       </c>
       <c r="D66" s="21" t="s">
@@ -2740,28 +3055,28 @@
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6">
       <c r="A67" s="5"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
       <c r="D67" s="22"/>
     </row>
-    <row r="68" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:6" ht="15.75" thickBot="1">
       <c r="A68" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="23"/>
     </row>
-    <row r="69" spans="1:6" ht="340.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="340.5" customHeight="1">
       <c r="A69" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="18" t="s">
         <v>211</v>
       </c>
       <c r="D69" s="21" t="s">
@@ -2774,28 +3089,28 @@
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6">
       <c r="A70" s="5"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="22"/>
     </row>
-    <row r="71" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" ht="15.75" thickBot="1">
       <c r="A71" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="23"/>
     </row>
-    <row r="72" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="409.6" customHeight="1">
       <c r="A72" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="18" t="s">
         <v>217</v>
       </c>
       <c r="D72" s="9" t="s">
@@ -2808,64 +3123,64 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6">
       <c r="A73" s="5"/>
       <c r="B73" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="C73" s="18"/>
+      <c r="C73" s="19"/>
       <c r="D73" s="9"/>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="30">
       <c r="A74" s="5" t="s">
         <v>212</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C74" s="18"/>
+      <c r="C74" s="19"/>
       <c r="D74" s="9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6">
       <c r="A75" s="11"/>
       <c r="B75" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C75" s="18"/>
+      <c r="C75" s="19"/>
       <c r="D75" s="9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6">
       <c r="A76" s="11"/>
       <c r="B76" s="7"/>
-      <c r="C76" s="18"/>
+      <c r="C76" s="19"/>
       <c r="D76" s="9" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6">
       <c r="A77" s="11"/>
       <c r="B77" s="13"/>
-      <c r="C77" s="18"/>
+      <c r="C77" s="19"/>
       <c r="D77" s="9"/>
     </row>
-    <row r="78" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:6" ht="15.75" thickBot="1">
       <c r="A78" s="12"/>
       <c r="B78" s="8"/>
-      <c r="C78" s="19"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="15"/>
     </row>
-    <row r="79" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="409.6" customHeight="1">
       <c r="A79" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="18" t="s">
         <v>224</v>
       </c>
       <c r="D79" s="21" t="s">
@@ -2878,28 +3193,28 @@
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6">
       <c r="A80" s="5"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
       <c r="D80" s="22"/>
     </row>
-    <row r="81" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:6" ht="15.75" thickBot="1">
       <c r="A81" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
       <c r="D81" s="23"/>
     </row>
-    <row r="82" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" ht="30">
       <c r="A82" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B82" s="20" t="s">
+      <c r="B82" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="18" t="s">
         <v>228</v>
       </c>
       <c r="D82" s="21" t="s">
@@ -2912,28 +3227,28 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6">
       <c r="A83" s="5"/>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
       <c r="D83" s="22"/>
     </row>
-    <row r="84" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:6" ht="15.75" thickBot="1">
       <c r="A84" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
       <c r="D84" s="23"/>
     </row>
-    <row r="85" spans="1:6" ht="247.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" ht="247.5" customHeight="1">
       <c r="A85" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="C85" s="20" t="s">
+      <c r="C85" s="18" t="s">
         <v>231</v>
       </c>
       <c r="D85" s="21" t="s">
@@ -2946,28 +3261,28 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6">
       <c r="A86" s="5"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
       <c r="D86" s="22"/>
     </row>
-    <row r="87" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:6" ht="15.75" thickBot="1">
       <c r="A87" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
       <c r="D87" s="23"/>
     </row>
-    <row r="88" spans="1:6" ht="309.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" ht="309.60000000000002" customHeight="1">
       <c r="A88" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B88" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C88" s="18" t="s">
         <v>234</v>
       </c>
       <c r="D88" s="21" t="s">
@@ -2980,28 +3295,28 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6">
       <c r="A89" s="5"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
       <c r="D89" s="22"/>
     </row>
-    <row r="90" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:6" ht="15.75" thickBot="1">
       <c r="A90" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
       <c r="D90" s="23"/>
     </row>
-    <row r="91" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" ht="409.6" customHeight="1">
       <c r="A91" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B91" s="20" t="s">
+      <c r="B91" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="18" t="s">
         <v>236</v>
       </c>
       <c r="D91" s="21" t="s">
@@ -3014,28 +3329,28 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6">
       <c r="A92" s="5"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="22"/>
     </row>
-    <row r="93" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:6" ht="15.75" thickBot="1">
       <c r="A93" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B93" s="19"/>
-      <c r="C93" s="19"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="20"/>
       <c r="D93" s="23"/>
     </row>
-    <row r="94" spans="1:6" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" ht="231.95" customHeight="1">
       <c r="A94" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B94" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C94" s="18" t="s">
         <v>238</v>
       </c>
       <c r="D94" s="21" t="s">
@@ -3048,28 +3363,28 @@
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6">
       <c r="A95" s="5"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="19"/>
       <c r="D95" s="22"/>
     </row>
-    <row r="96" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:6" ht="15.75" thickBot="1">
       <c r="A96" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B96" s="19"/>
-      <c r="C96" s="19"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="20"/>
       <c r="D96" s="23"/>
     </row>
-    <row r="97" spans="1:6" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" ht="231.95" customHeight="1">
       <c r="A97" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B97" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C97" s="18" t="s">
         <v>238</v>
       </c>
       <c r="D97" s="21" t="s">
@@ -3082,21 +3397,21 @@
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6">
       <c r="A98" s="5"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
       <c r="D98" s="22"/>
     </row>
-    <row r="99" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:6" ht="15.75" thickBot="1">
       <c r="A99" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B99" s="19"/>
-      <c r="C99" s="19"/>
+      <c r="B99" s="20"/>
+      <c r="C99" s="20"/>
       <c r="D99" s="23"/>
     </row>
-    <row r="100" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6">
       <c r="A100" s="5" t="s">
         <v>48</v>
       </c>
@@ -3116,7 +3431,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6">
       <c r="A101" s="5"/>
       <c r="B101" s="7" t="s">
         <v>121</v>
@@ -3128,7 +3443,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6">
       <c r="A102" s="5" t="s">
         <v>240</v>
       </c>
@@ -3140,7 +3455,7 @@
       </c>
       <c r="D102" s="9"/>
     </row>
-    <row r="103" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6">
       <c r="A103" s="11"/>
       <c r="B103" s="7" t="s">
         <v>243</v>
@@ -3152,7 +3467,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6">
       <c r="A104" s="11"/>
       <c r="B104" s="7" t="s">
         <v>244</v>
@@ -3162,7 +3477,7 @@
       </c>
       <c r="D104" s="14"/>
     </row>
-    <row r="105" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6">
       <c r="A105" s="11"/>
       <c r="B105" s="7" t="s">
         <v>245</v>
@@ -3172,7 +3487,7 @@
       </c>
       <c r="D105" s="14"/>
     </row>
-    <row r="106" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6">
       <c r="A106" s="11"/>
       <c r="B106" s="7" t="s">
         <v>246</v>
@@ -3182,13 +3497,13 @@
       </c>
       <c r="D106" s="14"/>
     </row>
-    <row r="107" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6">
       <c r="A107" s="11"/>
       <c r="B107" s="13"/>
       <c r="C107" s="7"/>
       <c r="D107" s="14"/>
     </row>
-    <row r="108" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6">
       <c r="A108" s="11"/>
       <c r="B108" s="13"/>
       <c r="C108" s="7" t="s">
@@ -3196,19 +3511,19 @@
       </c>
       <c r="D108" s="14"/>
     </row>
-    <row r="109" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6">
       <c r="A109" s="11"/>
       <c r="B109" s="13"/>
       <c r="C109" s="14"/>
       <c r="D109" s="14"/>
     </row>
-    <row r="110" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6">
       <c r="A110" s="11"/>
       <c r="B110" s="13"/>
       <c r="C110" s="7"/>
       <c r="D110" s="14"/>
     </row>
-    <row r="111" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" ht="15.75">
       <c r="A111" s="11"/>
       <c r="B111" s="13"/>
       <c r="C111" s="7" t="s">
@@ -3216,13 +3531,13 @@
       </c>
       <c r="D111" s="14"/>
     </row>
-    <row r="112" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:6" ht="16.5" thickBot="1">
       <c r="A112" s="12"/>
       <c r="B112" s="8"/>
       <c r="C112" s="17"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" ht="30">
       <c r="A113" s="5" t="s">
         <v>50</v>
       </c>
@@ -3242,7 +3557,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6">
       <c r="A114" s="5"/>
       <c r="B114" s="7" t="s">
         <v>121</v>
@@ -3252,7 +3567,7 @@
       </c>
       <c r="D114" s="9"/>
     </row>
-    <row r="115" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" ht="30">
       <c r="A115" s="5" t="s">
         <v>256</v>
       </c>
@@ -3266,7 +3581,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6">
       <c r="A116" s="11"/>
       <c r="B116" s="7" t="s">
         <v>127</v>
@@ -3276,7 +3591,7 @@
       </c>
       <c r="D116" s="14"/>
     </row>
-    <row r="117" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6">
       <c r="A117" s="11"/>
       <c r="B117" s="7" t="s">
         <v>258</v>
@@ -3286,7 +3601,7 @@
       </c>
       <c r="D117" s="14"/>
     </row>
-    <row r="118" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6">
       <c r="A118" s="11"/>
       <c r="B118" s="7" t="s">
         <v>193</v>
@@ -3296,7 +3611,7 @@
       </c>
       <c r="D118" s="14"/>
     </row>
-    <row r="119" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6">
       <c r="A119" s="11"/>
       <c r="B119" s="7" t="s">
         <v>160</v>
@@ -3306,41 +3621,31 @@
       </c>
       <c r="D119" s="14"/>
     </row>
-    <row r="120" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6">
       <c r="A120" s="11"/>
       <c r="B120" s="13"/>
       <c r="C120" s="7"/>
       <c r="D120" s="14"/>
     </row>
-    <row r="121" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:6" ht="15.75" thickBot="1">
       <c r="A121" s="12"/>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6">
       <c r="A122" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="B91:B93"/>
-    <mergeCell ref="C91:C93"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="C82:C84"/>
-    <mergeCell ref="D82:D84"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="C60:C65"/>
+    <mergeCell ref="D60:D65"/>
     <mergeCell ref="B69:B71"/>
     <mergeCell ref="C69:C71"/>
     <mergeCell ref="D69:D71"/>
@@ -3348,14 +3653,24 @@
     <mergeCell ref="B79:B81"/>
     <mergeCell ref="C79:C81"/>
     <mergeCell ref="D79:D81"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="C60:C65"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="C85:C87"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="B91:B93"/>
+    <mergeCell ref="C91:C93"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="D97:D99"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3363,23 +3678,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="E12" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="93.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="206.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.7265625" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="206.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3405,7 +3720,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3429,7 +3744,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3453,7 +3768,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3477,7 +3792,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3501,7 +3816,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -3525,7 +3840,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3552,7 +3867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -3576,7 +3891,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3603,7 +3918,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -3630,7 +3945,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -3657,7 +3972,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -3684,7 +3999,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3708,7 +4023,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -3735,7 +4050,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -3759,7 +4074,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3783,7 +4098,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -3807,7 +4122,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -3834,7 +4149,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -3861,7 +4176,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -3888,7 +4203,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3912,7 +4227,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -3936,7 +4251,7 @@
         <v>success</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -3963,7 +4278,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -3990,7 +4305,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -4017,7 +4332,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -4044,7 +4359,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -4069,6 +4384,30 @@
       </c>
       <c r="H27" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>272</v>
+      </c>
+      <c r="B28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" t="s">
+        <v>274</v>
+      </c>
+      <c r="D28" t="s">
+        <v>275</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="str">
+        <f>Tabela1[[#This Row],[NaLIR]]</f>
+        <v>success</v>
       </c>
     </row>
   </sheetData>

</xml_diff>